<commit_message>
Ajout du coût des plaquettes et DHT
Le coût réel des plaquettes et des capteurs de température + humidité
</commit_message>
<xml_diff>
--- a/cociclo_placeCommune/cociclo_2016_BOM.xlsx
+++ b/cociclo_placeCommune/cociclo_2016_BOM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Cociclo 2016</t>
   </si>
@@ -100,9 +100,6 @@
   </si>
   <si>
     <t>Capteur de Temp et Humidité</t>
-  </si>
-  <si>
-    <t>(sera 2-3$)</t>
   </si>
   <si>
     <t>Place commune</t>
@@ -541,7 +538,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -553,7 +550,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -592,7 +589,7 @@
         <v>8</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -660,11 +657,15 @@
       <c r="D12" t="s">
         <v>24</v>
       </c>
-      <c r="F12" t="s">
-        <v>27</v>
+      <c r="E12">
+        <v>225</v>
+      </c>
+      <c r="F12">
+        <v>100</v>
       </c>
       <c r="G12">
-        <v>0</v>
+        <f>E12/F12</f>
+        <v>2.25</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -673,7 +674,7 @@
       </c>
       <c r="G14">
         <f>SUM(G4:G13)</f>
-        <v>15.609999999999998</v>
+        <v>20.86</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -690,7 +691,7 @@
       </c>
       <c r="G16" s="1">
         <f>G15*G14</f>
-        <v>20.292999999999999</v>
+        <v>27.117999999999999</v>
       </c>
     </row>
     <row r="17" spans="6:7">
@@ -707,7 +708,7 @@
       </c>
       <c r="G18" s="3">
         <f>SUM(G16:G17)</f>
-        <v>22.292999999999999</v>
+        <v>29.117999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>